<commit_message>
changed fraction poor to 0.1%
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2017Sep/regions/InputForCode_Mjini_Magharibi.xlsx
+++ b/input_spreadsheets/Tanzania/2017Sep/regions/InputForCode_Mjini_Magharibi.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Tanzania application/Input sheets Tanzania/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9280" yWindow="460" windowWidth="16320" windowHeight="14260" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="-71760" yWindow="-4080" windowWidth="27580" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -38,13 +33,13 @@
     <sheet name="Interventions mortality eff" sheetId="24" r:id="rId24"/>
     <sheet name="Interventions incidence eff" sheetId="25" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -2911,16 +2906,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2928,7 +2923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -2936,7 +2931,7 @@
         <v>114744.07585648738</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -2944,7 +2939,7 @@
         <v>21960.626638696664</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -2952,7 +2947,7 @@
         <v>25821.007749825007</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>71</v>
       </c>
@@ -2960,15 +2955,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>70</v>
       </c>
       <c r="B6" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>72</v>
       </c>
@@ -2980,6 +2975,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2991,12 +2991,12 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>46</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>47</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>48</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>46</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>47</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>48</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>46</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>46</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>47</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>48</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="5" t="s">
         <v>46</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>47</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>48</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="B23" s="5" t="s">
         <v>46</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="B24" s="5" t="s">
         <v>47</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="B25" s="5" t="s">
         <v>48</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="B27" s="5" t="s">
         <v>46</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="B28" s="5" t="s">
         <v>47</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="B29" s="5" t="s">
         <v>48</v>
       </c>
@@ -3602,6 +3602,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3613,13 +3618,13 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -3636,7 +3641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
@@ -3655,7 +3660,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>21</v>
       </c>
@@ -3674,7 +3679,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>22</v>
       </c>
@@ -3693,7 +3698,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -3712,7 +3717,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>27</v>
       </c>
@@ -3731,7 +3736,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>28</v>
       </c>
@@ -3750,7 +3755,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>54</v>
       </c>
@@ -3769,7 +3774,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>31</v>
       </c>
@@ -3788,113 +3793,118 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="B14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1">
       <c r="B17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:7" ht="15.75" customHeight="1">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:7" ht="15.75" customHeight="1">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:7" ht="15.75" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:7" ht="15.75" customHeight="1">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:7" ht="15.75" customHeight="1">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:7" ht="15.75" customHeight="1">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:7" ht="15.75" customHeight="1">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:7" ht="15.75" customHeight="1">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:7" ht="15.75" customHeight="1">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:7" ht="15.75" customHeight="1">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3906,9 +3916,9 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -3922,7 +3932,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="5">
         <v>45</v>
       </c>
@@ -3938,6 +3948,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3947,12 +3962,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>55</v>
       </c>
@@ -3972,7 +3987,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>45</v>
       </c>
@@ -3992,7 +4007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
@@ -4012,7 +4027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>47</v>
       </c>
@@ -4032,7 +4047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>48</v>
       </c>
@@ -4054,6 +4069,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4065,9 +4085,9 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>49</v>
       </c>
@@ -4087,7 +4107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -4109,6 +4129,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4120,9 +4145,9 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>53</v>
       </c>
@@ -4136,7 +4161,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -4152,6 +4177,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4163,12 +4193,12 @@
       <selection activeCell="E30" sqref="E29:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -4188,7 +4218,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>73</v>
       </c>
@@ -4208,7 +4238,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -4216,7 +4246,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -4224,7 +4254,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -4235,6 +4265,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4246,12 +4281,12 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="70.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>78</v>
       </c>
@@ -4271,7 +4306,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>57</v>
       </c>
@@ -4291,7 +4326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>58</v>
       </c>
@@ -4311,7 +4346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
@@ -4331,7 +4366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>60</v>
       </c>
@@ -4353,6 +4388,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4364,13 +4404,13 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="43.1640625" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -4390,7 +4430,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="14">
       <c r="A2" s="5" t="s">
         <v>74</v>
       </c>
@@ -4410,7 +4450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="14">
       <c r="A3" s="5" t="s">
         <v>75</v>
       </c>
@@ -4430,7 +4470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -4440,6 +4480,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4449,12 +4494,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -4471,7 +4516,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="14">
       <c r="A2" s="11" t="s">
         <v>45</v>
       </c>
@@ -4488,14 +4533,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -4504,6 +4549,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4515,13 +4565,13 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4529,7 +4579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="4">
         <v>2017</v>
       </c>
@@ -4537,7 +4587,7 @@
         <v>22384.99</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="4">
         <v>2018</v>
       </c>
@@ -4545,7 +4595,7 @@
         <v>22809.350000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="4">
         <v>2019</v>
       </c>
@@ -4553,7 +4603,7 @@
         <v>23339.8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="4">
         <v>2020</v>
       </c>
@@ -4561,7 +4611,7 @@
         <v>23764.16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="4">
         <v>2021</v>
       </c>
@@ -4569,7 +4619,7 @@
         <v>24188.52</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="4">
         <v>2022</v>
       </c>
@@ -4577,7 +4627,7 @@
         <v>24718.97</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
       <c r="A8" s="4">
         <v>2023</v>
       </c>
@@ -4585,7 +4635,7 @@
         <v>25249.420000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
       <c r="A9" s="4">
         <v>2024</v>
       </c>
@@ -4593,7 +4643,7 @@
         <v>25673.780000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1">
       <c r="A10" s="4">
         <v>2025</v>
       </c>
@@ -4601,7 +4651,7 @@
         <v>26310.32</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
       <c r="A11" s="4">
         <v>2026</v>
       </c>
@@ -4609,7 +4659,7 @@
         <v>26840.77</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="4">
         <v>2027</v>
       </c>
@@ -4617,7 +4667,7 @@
         <v>27371.22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
       <c r="A13" s="4">
         <v>2028</v>
       </c>
@@ -4625,7 +4675,7 @@
         <v>27901.670000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
       <c r="A14" s="4">
         <v>2029</v>
       </c>
@@ -4633,7 +4683,7 @@
         <v>28538.210000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1">
       <c r="A15" s="4">
         <v>2030</v>
       </c>
@@ -4643,6 +4693,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4654,7 +4709,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.83203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -4662,7 +4717,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -4676,7 +4731,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -4693,7 +4748,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>75</v>
       </c>
@@ -4710,7 +4765,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>76</v>
       </c>
@@ -4727,7 +4782,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>74</v>
       </c>
@@ -4744,7 +4799,7 @@
       <c r="F5" s="14"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -4758,7 +4813,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -4775,7 +4830,7 @@
       <c r="F7" s="14"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>80</v>
       </c>
@@ -4792,77 +4847,77 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:3" ht="15.75" customHeight="1">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:3" ht="15.75" customHeight="1">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:3" ht="15.75" customHeight="1">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:3" ht="15.75" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:3" ht="15.75" customHeight="1">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:3" ht="15.75" customHeight="1">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:3" ht="15.75" customHeight="1">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:3" ht="15.75" customHeight="1">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
@@ -4870,6 +4925,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4881,7 +4941,7 @@
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.6640625" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
@@ -4891,7 +4951,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -4916,7 +4976,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -4939,7 +4999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>75</v>
       </c>
@@ -4962,7 +5022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>76</v>
       </c>
@@ -4974,11 +5034,11 @@
       </c>
       <c r="D4" s="4">
         <f>demographics!$B$6</f>
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E4" s="4">
         <f>demographics!$B$6</f>
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
@@ -4987,7 +5047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>74</v>
       </c>
@@ -5010,7 +5070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -5031,10 +5091,10 @@
       </c>
       <c r="G6" s="4">
         <f>demographics!$B$6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -5057,7 +5117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>80</v>
       </c>
@@ -5080,72 +5140,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="B9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="B10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="B11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:3" ht="15.75" customHeight="1">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:3" ht="15.75" customHeight="1">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:3" ht="15.75" customHeight="1">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:3" ht="15.75" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:3" ht="15.75" customHeight="1">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:3" ht="15.75" customHeight="1">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:3" ht="15.75" customHeight="1">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
@@ -5153,6 +5213,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5164,12 +5229,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -5189,7 +5254,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -5209,17 +5274,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="15">
         <f>demographics!$B$5 * 'Interventions target population'!$G$6</f>
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D3" s="15">
         <f>demographics!$B$5 * 'Interventions target population'!$G$6</f>
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E3" s="15">
         <v>0</v>
@@ -5228,7 +5293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -5248,7 +5313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="B5" t="s">
         <v>69</v>
       </c>
@@ -5265,14 +5330,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="5"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -5282,6 +5347,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5293,12 +5363,12 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -5321,7 +5391,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -5344,7 +5414,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
@@ -5364,7 +5434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>80</v>
       </c>
@@ -5387,7 +5457,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -5411,6 +5481,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5422,12 +5497,12 @@
       <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -5450,7 +5525,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -5473,7 +5548,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
@@ -5493,7 +5568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>80</v>
       </c>
@@ -5519,7 +5594,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -5543,6 +5618,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5554,12 +5634,12 @@
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -5582,7 +5662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -5605,7 +5685,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
@@ -5625,7 +5705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>80</v>
       </c>
@@ -5651,7 +5731,7 @@
         <v>0.496</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -5675,6 +5755,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5686,9 +5771,9 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -5699,7 +5784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="29">
         <v>33</v>
       </c>
@@ -5714,6 +5799,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5725,12 +5815,12 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -5750,7 +5840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5770,7 +5860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -5790,7 +5880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -5810,7 +5900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -5830,7 +5920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -5850,7 +5940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -5870,7 +5960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -5890,7 +5980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -5910,7 +6000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -5930,7 +6020,7 @@
         <v>0.1368</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -5950,7 +6040,7 @@
         <v>0.20660000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -5970,7 +6060,7 @@
         <v>2.1100000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -5990,7 +6080,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -6010,7 +6100,7 @@
         <v>8.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -6030,7 +6120,7 @@
         <v>2.86E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -6050,7 +6140,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -6070,7 +6160,7 @@
         <v>0.13589999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -6097,6 +6187,11 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6104,13 +6199,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -6133,7 +6228,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -6161,7 +6256,7 @@
         <v>45.310671653201773</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -6186,7 +6281,7 @@
         <v>35.805462067728456</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
@@ -6206,7 +6301,7 @@
         <v>11.996686791890284</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
@@ -6226,7 +6321,7 @@
         <v>6.8871794871794858</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>35</v>
       </c>
@@ -6249,7 +6344,7 @@
         <v>48.515000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
@@ -6269,7 +6364,7 @@
         <v>48.515000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
@@ -6289,7 +6384,7 @@
         <v>2.2399999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
@@ -6309,7 +6404,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>44</v>
       </c>
@@ -6332,7 +6427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>46</v>
       </c>
@@ -6352,7 +6447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
@@ -6372,7 +6467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
@@ -6400,6 +6495,11 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6411,9 +6511,9 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
@@ -6424,7 +6524,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="30">
         <v>8.8255813953488377E-3</v>
       </c>
@@ -6437,6 +6537,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6448,9 +6553,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>49</v>
       </c>
@@ -6470,7 +6575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -6490,7 +6595,7 @@
         <v>1.6089788135593222</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
@@ -6514,6 +6619,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6523,9 +6633,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -6548,7 +6658,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -6571,7 +6681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -6591,7 +6701,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
@@ -6611,7 +6721,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
@@ -6631,7 +6741,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -6654,7 +6764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
@@ -6674,7 +6784,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
@@ -6694,7 +6804,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
@@ -6714,7 +6824,7 @@
         <v>6.39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -6737,7 +6847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
@@ -6757,7 +6867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
@@ -6777,7 +6887,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
@@ -6797,7 +6907,7 @@
         <v>6.01</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -6820,7 +6930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
@@ -6840,7 +6950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
@@ -6860,7 +6970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
@@ -6880,7 +6990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -6903,7 +7013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
@@ -6923,7 +7033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
@@ -6943,7 +7053,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
@@ -6965,6 +7075,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6974,9 +7089,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -6999,7 +7114,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -7022,7 +7137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -7042,7 +7157,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
@@ -7062,7 +7177,7 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
@@ -7082,7 +7197,7 @@
         <v>12.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -7105,7 +7220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
@@ -7125,7 +7240,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
@@ -7145,7 +7260,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
@@ -7165,7 +7280,7 @@
         <v>9.68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -7188,7 +7303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
@@ -7208,7 +7323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
@@ -7228,7 +7343,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
@@ -7248,7 +7363,7 @@
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -7271,7 +7386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
@@ -7291,7 +7406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
@@ -7311,7 +7426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
@@ -7331,7 +7446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -7354,7 +7469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
@@ -7374,7 +7489,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
@@ -7394,7 +7509,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
@@ -7416,5 +7531,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>